<commit_message>
add master data and python utility
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\masterdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ACF9C6-CD0E-4649-B0AC-26C76F66FCC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF58E23-F4CA-4BFF-9782-4D30407C650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="36">
   <si>
     <t>lang_code</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>000</t>
+  </si>
+  <si>
+    <t>hin</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -192,7 +198,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,19 +512,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.44140625" style="1"/>
-    <col min="5" max="5" width="8.5546875" style="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,1143 +544,2285 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" t="s">
         <v>25</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" t="s">
         <v>25</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" t="s">
         <v>25</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" t="s">
         <v>25</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
         <v>13</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" t="s">
         <v>15</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" t="s">
         <v>25</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="4" t="s">
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" t="s">
         <v>25</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="4" t="s">
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" s="4" t="s">
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" s="4" t="s">
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" s="4" t="s">
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" s="4" t="s">
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="4" t="s">
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>34</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>34</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>34</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>34</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" t="s">
+        <v>13</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>34</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>34</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>34</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" t="s">
+        <v>13</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>34</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>34</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>34</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>34</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C107" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" t="s">
+        <v>13</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C108" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>34</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C109" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" t="s">
+        <v>25</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>34</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>34</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C111" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>34</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
+        <v>25</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>34</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>34</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>34</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>34</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" t="s">
+        <v>25</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>34</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>34</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>34</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C120" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>34</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" t="s">
+        <v>24</v>
+      </c>
+      <c r="D121" t="s">
+        <v>25</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>34</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>34</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>34</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>34</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C125" t="s">
+        <v>24</v>
+      </c>
+      <c r="D125" t="s">
+        <v>25</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>34</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>34</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C127" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>34</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" t="s">
+        <v>24</v>
+      </c>
+      <c r="D128" t="s">
+        <v>25</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>34</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>34</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C130" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>34</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" t="s">
+        <v>11</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>34</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" t="s">
+        <v>11</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>34</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C133" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C134" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134" t="s">
+        <v>11</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>34</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C135" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H135" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save manual changes made in database to mosip-data repository
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosip\CIV\CODE\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-mec\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA79900-233F-46B7-9F08-262DB8DA9791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C089151C-884D-4B13-B8B4-002B40F317FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="34">
   <si>
     <t>lang_code</t>
   </si>
@@ -67,9 +67,6 @@
     <t>DOC007</t>
   </si>
   <si>
-    <t>POB</t>
-  </si>
-  <si>
     <t>DOC008</t>
   </si>
   <si>
@@ -82,33 +79,6 @@
     <t>DOC010</t>
   </si>
   <si>
-    <t>POA</t>
-  </si>
-  <si>
-    <t>DOC011</t>
-  </si>
-  <si>
-    <t>DOC012</t>
-  </si>
-  <si>
-    <t>DOC013</t>
-  </si>
-  <si>
-    <t>DOC014</t>
-  </si>
-  <si>
-    <t>POC</t>
-  </si>
-  <si>
-    <t>DOC015</t>
-  </si>
-  <si>
-    <t>DOC016</t>
-  </si>
-  <si>
-    <t>DOC017</t>
-  </si>
-  <si>
     <t>POM</t>
   </si>
   <si>
@@ -119,6 +89,42 @@
   </si>
   <si>
     <t>DOC005</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
   </si>
 </sst>
 </file>
@@ -461,19 +467,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -498,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -515,13 +521,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -532,13 +538,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -549,13 +555,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
@@ -566,13 +572,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -583,13 +589,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
@@ -600,13 +606,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
@@ -617,13 +623,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -634,10 +640,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>17</v>
@@ -651,13 +657,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -668,10 +674,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
@@ -685,13 +691,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
@@ -702,13 +708,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
@@ -719,13 +725,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
@@ -736,13 +742,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
@@ -753,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
@@ -770,13 +776,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
@@ -787,15 +793,865 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>